<commit_message>
Actualizacion platina y gabinete
</commit_message>
<xml_diff>
--- a/Formulacion.xlsx
+++ b/Formulacion.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CETI\Proyecto\Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A99F6B77-C35C-4FAC-9917-3ADA8263ADAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2233C297-846F-4849-84C8-E4B4F8B1FE8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Control-Incinerador PLASTIRAL" sheetId="1" r:id="rId1"/>
@@ -890,12 +890,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDBE9F7"/>
-        <bgColor rgb="FFDBE9F7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFD9F2D0"/>
         <bgColor rgb="FFD9F2D0"/>
       </patternFill>
@@ -939,6 +933,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFDBE9F7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor rgb="FFDBE9F7"/>
       </patternFill>
     </fill>
@@ -1031,20 +1031,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1066,23 +1063,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1090,15 +1095,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1318,8 +1318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:O1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:D15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -1341,35 +1341,35 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="30" customHeight="1">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="25"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="26"/>
     </row>
     <row r="3" spans="2:15" ht="33.75" customHeight="1">
-      <c r="B3" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="25"/>
-      <c r="M3" s="15" t="s">
+      <c r="B3" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="26"/>
+      <c r="M3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="N3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="14" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1377,10 +1377,10 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="25"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="2" t="s">
         <v>7</v>
       </c>
@@ -1396,803 +1396,803 @@
       <c r="I4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="15" t="s">
+      <c r="M4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="14" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="33.75" customHeight="1">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="25"/>
-      <c r="E5" s="5"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="3">
         <v>1</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="M5" s="15" t="s">
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="M5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="15" t="s">
+      <c r="N5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:15" ht="28.5" customHeight="1">
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="5"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="M6" s="15" t="s">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="M6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N6" s="16" t="s">
+      <c r="N6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="15" t="s">
+      <c r="O6" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:15" ht="15.75">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="E7" s="5"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
     </row>
     <row r="8" spans="2:15" ht="15.75">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="5"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
     </row>
     <row r="9" spans="2:15" ht="15.75">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="5"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="4"/>
       <c r="F9" s="3">
         <v>2</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="31" t="s">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="M9" s="16"/>
+      <c r="N9" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="O9" s="31"/>
+      <c r="O9" s="24"/>
     </row>
     <row r="10" spans="2:15" ht="15.75">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="25"/>
-      <c r="E10" s="5"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="4"/>
       <c r="F10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="31" t="s">
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="24" t="s">
         <v>256</v>
       </c>
-      <c r="O10" s="31"/>
+      <c r="O10" s="24"/>
     </row>
     <row r="11" spans="2:15" ht="15.75">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="25"/>
-      <c r="E11" s="5"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="4"/>
       <c r="F11" s="3">
         <v>1</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="M11" s="19"/>
-      <c r="N11" s="31"/>
-      <c r="O11" s="31"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="M11" s="18"/>
+      <c r="N11" s="24"/>
+      <c r="O11" s="24"/>
     </row>
     <row r="12" spans="2:15" ht="15.75">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="5"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="31" t="s">
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="24" t="s">
         <v>258</v>
       </c>
-      <c r="O12" s="31"/>
+      <c r="O12" s="24"/>
     </row>
     <row r="13" spans="2:15" ht="15.75">
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="25"/>
-      <c r="E13" s="5"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
     </row>
     <row r="14" spans="2:15" ht="15.75">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="5"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="3">
         <v>3</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
     </row>
     <row r="15" spans="2:15" ht="15.75">
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="25" t="s">
         <v>270</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="5"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="4"/>
       <c r="F15" s="3">
         <v>1</v>
       </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
     </row>
     <row r="16" spans="2:15" ht="15.75">
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="25" t="s">
         <v>269</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="5"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="3">
         <v>0</v>
       </c>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
     </row>
     <row r="17" spans="2:9" ht="15.75">
-      <c r="B17" s="33" t="s">
+      <c r="B17" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="25" t="s">
         <v>268</v>
       </c>
-      <c r="D17" s="25"/>
-      <c r="E17" s="5"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="4"/>
       <c r="F17" s="3">
         <v>1</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
     </row>
     <row r="18" spans="2:9" ht="15.75">
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="5"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="3">
         <v>1</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
     </row>
     <row r="19" spans="2:9" ht="15.75">
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C19" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="5"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="3">
         <v>1</v>
       </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
     </row>
     <row r="20" spans="2:9" ht="15.75">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="30"/>
-      <c r="E20" s="5"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="3">
         <v>2</v>
       </c>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
     </row>
     <row r="21" spans="2:9" ht="15.75">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="D21" s="25"/>
-      <c r="E21" s="6"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="3">
         <v>1</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
     </row>
     <row r="22" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="6"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="3">
         <v>3</v>
       </c>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
     <row r="23" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="D23" s="25"/>
-      <c r="E23" s="6"/>
+      <c r="D23" s="26"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="3">
         <v>1</v>
       </c>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="25"/>
-      <c r="E24" s="6"/>
+      <c r="D24" s="26"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="3">
         <v>2</v>
       </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
     </row>
     <row r="25" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="6"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="5"/>
       <c r="F25" s="3">
         <v>2</v>
       </c>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
     </row>
     <row r="26" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="25"/>
-      <c r="E26" s="6"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="5"/>
       <c r="F26" s="3">
         <v>1</v>
       </c>
-      <c r="G26" s="6"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="6"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
     </row>
     <row r="27" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B27" s="20" t="s">
+      <c r="B27" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="6"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="5"/>
       <c r="F27" s="3">
         <v>1</v>
       </c>
-      <c r="G27" s="6"/>
-      <c r="H27" s="6"/>
-      <c r="I27" s="6"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
     </row>
     <row r="28" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="25" t="s">
         <v>261</v>
       </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="6"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="5"/>
       <c r="F28" s="3">
         <v>1</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6"/>
-      <c r="I28" s="6"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="25" t="s">
         <v>262</v>
       </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="6"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="5"/>
       <c r="F29" s="3">
         <v>1</v>
       </c>
-      <c r="G29" s="6"/>
-      <c r="H29" s="6"/>
-      <c r="I29" s="6"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
     </row>
     <row r="30" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="6"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="5"/>
       <c r="F30" s="3">
         <v>1</v>
       </c>
-      <c r="G30" s="6"/>
-      <c r="H30" s="6"/>
-      <c r="I30" s="6"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
     </row>
     <row r="31" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B31" s="21" t="s">
+      <c r="B31" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="6"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="5"/>
       <c r="F31" s="3">
         <v>1</v>
       </c>
-      <c r="G31" s="6"/>
-      <c r="H31" s="6"/>
-      <c r="I31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
     </row>
     <row r="32" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C32" s="24" t="s">
+      <c r="C32" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="D32" s="25"/>
-      <c r="E32" s="6"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="5"/>
       <c r="F32" s="3">
         <v>1</v>
       </c>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
     </row>
     <row r="33" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="25"/>
-      <c r="E33" s="6"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="3">
         <v>1</v>
       </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
     </row>
     <row r="34" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="6"/>
+      <c r="D34" s="26"/>
+      <c r="E34" s="5"/>
       <c r="F34" s="3">
         <v>1</v>
       </c>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
     </row>
     <row r="35" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C35" s="24" t="s">
+      <c r="C35" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="D35" s="25"/>
-      <c r="E35" s="6"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="5"/>
       <c r="F35" s="3">
         <v>1</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6"/>
-      <c r="I35" s="6"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
     </row>
     <row r="36" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="24" t="s">
+      <c r="C36" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="25"/>
-      <c r="E36" s="6"/>
+      <c r="D36" s="26"/>
+      <c r="E36" s="5"/>
       <c r="F36" s="3">
         <v>1</v>
       </c>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B37" s="8" t="s">
+      <c r="B37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C37" s="24" t="s">
+      <c r="C37" s="25" t="s">
         <v>266</v>
       </c>
-      <c r="D37" s="25"/>
-      <c r="E37" s="6"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="5"/>
       <c r="F37" s="3">
         <v>1</v>
       </c>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
     </row>
     <row r="38" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="24" t="s">
+      <c r="C38" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D38" s="25"/>
-      <c r="E38" s="6"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="5"/>
       <c r="F38" s="3">
         <v>1</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
     </row>
     <row r="39" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="C39" s="24" t="s">
+      <c r="C39" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D39" s="25"/>
-      <c r="E39" s="6"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="5"/>
       <c r="F39" s="3">
         <v>1</v>
       </c>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
     </row>
     <row r="40" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="24" t="s">
+      <c r="C40" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="25"/>
-      <c r="E40" s="6"/>
+      <c r="D40" s="26"/>
+      <c r="E40" s="5"/>
       <c r="F40" s="3">
         <v>1</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5"/>
+      <c r="I40" s="5"/>
     </row>
     <row r="41" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="C41" s="24" t="s">
+      <c r="C41" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="D41" s="25"/>
-      <c r="E41" s="6"/>
+      <c r="D41" s="26"/>
+      <c r="E41" s="5"/>
       <c r="F41" s="3">
         <v>1</v>
       </c>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="23" t="s">
         <v>260</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="25" t="s">
         <v>259</v>
       </c>
-      <c r="D42" s="25"/>
-      <c r="E42" s="6"/>
+      <c r="D42" s="26"/>
+      <c r="E42" s="5"/>
       <c r="F42" s="3">
         <v>2</v>
       </c>
-      <c r="G42" s="6"/>
-      <c r="H42" s="6"/>
-      <c r="I42" s="6"/>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5"/>
+      <c r="I42" s="5"/>
     </row>
     <row r="43" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C43" s="24" t="s">
+      <c r="C43" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="25"/>
-      <c r="E43" s="6"/>
+      <c r="D43" s="26"/>
+      <c r="E43" s="5"/>
       <c r="F43" s="3">
         <v>1</v>
       </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6"/>
-      <c r="I43" s="6"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
+      <c r="I43" s="5"/>
     </row>
     <row r="44" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B44" s="8"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="6"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="5"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6"/>
-      <c r="I44" s="6"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
     </row>
     <row r="45" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B45" s="8"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="6"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="5"/>
       <c r="F45" s="3"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
     </row>
     <row r="46" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B46" s="8"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="6"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="5"/>
       <c r="F46" s="3"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
     </row>
     <row r="47" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B47" s="10"/>
-      <c r="C47" s="10"/>
-      <c r="D47" s="10"/>
-      <c r="E47" s="10"/>
-      <c r="F47" s="10"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
     </row>
     <row r="48" spans="2:9" ht="15.75" customHeight="1">
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
     </row>
     <row r="49" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
-      <c r="E49" s="10"/>
-      <c r="F49" s="10"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
     </row>
     <row r="50" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B50" s="10"/>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
-      <c r="E50" s="10"/>
-      <c r="F50" s="10"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
     </row>
     <row r="51" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B51" s="10"/>
-      <c r="C51" s="10"/>
-      <c r="D51" s="10"/>
-      <c r="E51" s="10"/>
-      <c r="F51" s="10"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
     </row>
     <row r="52" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="10"/>
-      <c r="E52" s="10"/>
-      <c r="F52" s="10"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
     </row>
     <row r="53" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B53" s="10"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
     </row>
     <row r="54" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B54" s="10"/>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
-      <c r="E54" s="10"/>
-      <c r="F54" s="10"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
     </row>
     <row r="55" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="10"/>
-      <c r="E55" s="10"/>
-      <c r="F55" s="10"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
     </row>
     <row r="56" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B56" s="10"/>
-      <c r="C56" s="10"/>
-      <c r="D56" s="10"/>
-      <c r="E56" s="10"/>
-      <c r="F56" s="10"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="9"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
     </row>
     <row r="57" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B57" s="10"/>
-      <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="10"/>
-      <c r="F57" s="10"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="10"/>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="9"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
     </row>
     <row r="59" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
     </row>
     <row r="60" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B60" s="10"/>
-      <c r="C60" s="10"/>
-      <c r="D60" s="10"/>
-      <c r="E60" s="10"/>
-      <c r="F60" s="10"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
     </row>
     <row r="61" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="62" spans="2:6" ht="15.75" customHeight="1"/>
@@ -3137,6 +3137,39 @@
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
     <mergeCell ref="N12:O12"/>
     <mergeCell ref="N9:O9"/>
     <mergeCell ref="N10:O10"/>
@@ -3153,39 +3186,6 @@
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C32:D32"/>
     <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -3229,53 +3229,53 @@
       <c r="C3" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
-      <c r="R3" s="30"/>
-      <c r="S3" s="30"/>
-      <c r="T3" s="30"/>
-      <c r="U3" s="30"/>
-      <c r="V3" s="30"/>
-      <c r="W3" s="30"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="28"/>
+      <c r="V3" s="28"/>
+      <c r="W3" s="28"/>
     </row>
     <row r="4" spans="3:23">
       <c r="C4" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="11"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="10"/>
       <c r="K4" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="11"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="10"/>
       <c r="S4" s="32" t="s">
         <v>87</v>
       </c>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
     </row>
     <row r="5" spans="3:23">
       <c r="C5" s="1" t="s">
@@ -3343,7 +3343,7 @@
       <c r="D6" s="1">
         <v>3</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="11"/>
       <c r="K6" s="1" t="s">
         <v>94</v>
       </c>
@@ -3364,14 +3364,14 @@
       <c r="E7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="12">
         <v>45722</v>
       </c>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
       <c r="K7" s="1" t="s">
         <v>98</v>
       </c>
@@ -3395,14 +3395,14 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="12">
         <v>45722</v>
       </c>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
       <c r="K8" s="1" t="s">
         <v>102</v>
       </c>
@@ -3420,7 +3420,7 @@
       <c r="D9" s="1">
         <v>3</v>
       </c>
-      <c r="F9" s="12"/>
+      <c r="F9" s="11"/>
       <c r="K9" s="1" t="s">
         <v>105</v>
       </c>
@@ -3438,7 +3438,7 @@
       <c r="D10" s="1">
         <v>5</v>
       </c>
-      <c r="F10" s="12"/>
+      <c r="F10" s="11"/>
       <c r="K10" s="1" t="s">
         <v>108</v>
       </c>
@@ -3462,14 +3462,14 @@
       <c r="E11" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="F11" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="12">
         <v>45722</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
       <c r="K11" s="1" t="s">
         <v>113</v>
       </c>
@@ -3487,7 +3487,7 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="12"/>
+      <c r="F12" s="11"/>
       <c r="K12" s="1" t="s">
         <v>116</v>
       </c>
@@ -3508,14 +3508,14 @@
       <c r="E13" s="1">
         <v>3</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="13">
+      <c r="G13" s="12">
         <v>45722</v>
       </c>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
       <c r="K13" s="1" t="s">
         <v>120</v>
       </c>
@@ -3533,7 +3533,7 @@
       <c r="D14" s="1">
         <v>3</v>
       </c>
-      <c r="F14" s="12"/>
+      <c r="F14" s="11"/>
       <c r="K14" s="1" t="s">
         <v>123</v>
       </c>
@@ -3551,7 +3551,7 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-      <c r="F15" s="12"/>
+      <c r="F15" s="11"/>
       <c r="K15" s="1" t="s">
         <v>126</v>
       </c>
@@ -3569,7 +3569,7 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-      <c r="F16" s="12"/>
+      <c r="F16" s="11"/>
       <c r="K16" s="1" t="s">
         <v>129</v>
       </c>
@@ -3590,7 +3590,7 @@
       <c r="D17" s="1">
         <v>3</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="11"/>
       <c r="K17" s="1" t="s">
         <v>132</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="11"/>
       <c r="K18" s="1" t="s">
         <v>134</v>
       </c>
@@ -3626,14 +3626,14 @@
       <c r="E19" s="1">
         <v>1</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="12">
         <v>45722</v>
       </c>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
       <c r="K19" s="1" t="s">
         <v>137</v>
       </c>
@@ -3648,7 +3648,7 @@
       <c r="D20" s="1">
         <v>3</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="11"/>
       <c r="K20" s="1" t="s">
         <v>139</v>
       </c>
@@ -3663,7 +3663,7 @@
       <c r="D21" s="1">
         <v>3</v>
       </c>
-      <c r="F21" s="12"/>
+      <c r="F21" s="11"/>
       <c r="K21" s="1" t="s">
         <v>141</v>
       </c>
@@ -3678,7 +3678,7 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="F22" s="12"/>
+      <c r="F22" s="11"/>
       <c r="K22" s="1" t="s">
         <v>143</v>
       </c>
@@ -3693,7 +3693,7 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-      <c r="F23" s="12"/>
+      <c r="F23" s="11"/>
       <c r="K23" s="1" t="s">
         <v>145</v>
       </c>
@@ -3711,14 +3711,14 @@
       <c r="E24" s="1">
         <v>1</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="12">
         <v>45722</v>
       </c>
-      <c r="H24" s="13"/>
-      <c r="I24" s="13"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
       <c r="K24" s="1" t="s">
         <v>148</v>
       </c>
@@ -3733,7 +3733,7 @@
       <c r="D25" s="1">
         <v>5</v>
       </c>
-      <c r="F25" s="12"/>
+      <c r="F25" s="11"/>
       <c r="K25" s="1" t="s">
         <v>150</v>
       </c>
@@ -3751,7 +3751,7 @@
       <c r="D26" s="1">
         <v>3</v>
       </c>
-      <c r="F26" s="12"/>
+      <c r="F26" s="11"/>
       <c r="K26" s="1" t="s">
         <v>152</v>
       </c>
@@ -3766,7 +3766,7 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-      <c r="F27" s="12"/>
+      <c r="F27" s="11"/>
       <c r="K27" s="1" t="s">
         <v>154</v>
       </c>
@@ -3781,7 +3781,7 @@
       <c r="D28" s="1">
         <v>2</v>
       </c>
-      <c r="F28" s="12"/>
+      <c r="F28" s="11"/>
       <c r="K28" s="1" t="s">
         <v>156</v>
       </c>
@@ -3796,7 +3796,7 @@
       <c r="D29" s="1">
         <v>1</v>
       </c>
-      <c r="F29" s="12"/>
+      <c r="F29" s="11"/>
       <c r="K29" s="1" t="s">
         <v>158</v>
       </c>
@@ -3811,7 +3811,7 @@
       <c r="D30" s="1">
         <v>5</v>
       </c>
-      <c r="F30" s="12"/>
+      <c r="F30" s="11"/>
       <c r="K30" s="1" t="s">
         <v>160</v>
       </c>
@@ -3826,7 +3826,7 @@
       <c r="D31" s="1">
         <v>3</v>
       </c>
-      <c r="F31" s="12"/>
+      <c r="F31" s="11"/>
       <c r="K31" s="1" t="s">
         <v>162</v>
       </c>
@@ -3841,7 +3841,7 @@
       <c r="D32" s="1">
         <v>5</v>
       </c>
-      <c r="F32" s="12"/>
+      <c r="F32" s="11"/>
       <c r="K32" s="1" t="s">
         <v>164</v>
       </c>
@@ -3856,7 +3856,7 @@
       <c r="D33" s="1">
         <v>2</v>
       </c>
-      <c r="F33" s="12"/>
+      <c r="F33" s="11"/>
       <c r="K33" s="1" t="s">
         <v>166</v>
       </c>
@@ -3874,7 +3874,7 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
-      <c r="F34" s="12"/>
+      <c r="F34" s="11"/>
       <c r="K34" s="1" t="s">
         <v>168</v>
       </c>
@@ -3892,7 +3892,7 @@
       <c r="D35" s="1">
         <v>3</v>
       </c>
-      <c r="F35" s="12"/>
+      <c r="F35" s="11"/>
       <c r="K35" s="1" t="s">
         <v>170</v>
       </c>
@@ -3907,7 +3907,7 @@
       <c r="D36" s="1">
         <v>1</v>
       </c>
-      <c r="F36" s="12"/>
+      <c r="F36" s="11"/>
       <c r="K36" s="1" t="s">
         <v>172</v>
       </c>
@@ -3922,7 +3922,7 @@
       <c r="D37" s="1">
         <v>5</v>
       </c>
-      <c r="F37" s="12"/>
+      <c r="F37" s="11"/>
       <c r="K37" s="1" t="s">
         <v>174</v>
       </c>
@@ -3940,14 +3940,14 @@
       <c r="E38" s="1">
         <v>2</v>
       </c>
-      <c r="F38" s="12" t="s">
+      <c r="F38" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="12">
         <v>45722</v>
       </c>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
+      <c r="H38" s="12"/>
+      <c r="I38" s="12"/>
       <c r="K38" s="1" t="s">
         <v>176</v>
       </c>
@@ -3965,18 +3965,18 @@
       <c r="E39" s="1">
         <v>3</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="F39" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G39" s="13">
+      <c r="G39" s="12">
         <v>45722</v>
       </c>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
       <c r="K39" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="L39" s="14" t="s">
+      <c r="L39" s="13" t="s">
         <v>24</v>
       </c>
       <c r="N39" s="1" t="s">
@@ -3990,7 +3990,7 @@
       <c r="D40" s="1">
         <v>5</v>
       </c>
-      <c r="F40" s="12"/>
+      <c r="F40" s="11"/>
       <c r="K40" s="1" t="s">
         <v>181</v>
       </c>
@@ -4008,14 +4008,14 @@
       <c r="E41" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F41" s="12" t="s">
+      <c r="F41" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G41" s="13">
+      <c r="G41" s="12">
         <v>45722</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12"/>
       <c r="K41" s="1" t="s">
         <v>184</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-      <c r="F42" s="12"/>
+      <c r="F42" s="11"/>
       <c r="K42" s="1" t="s">
         <v>186</v>
       </c>
@@ -4048,14 +4048,14 @@
       <c r="E43" s="1">
         <v>1</v>
       </c>
-      <c r="F43" s="12" t="s">
+      <c r="F43" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="G43" s="13">
+      <c r="G43" s="12">
         <v>45722</v>
       </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
       <c r="K43" s="1" t="s">
         <v>188</v>
       </c>
@@ -4073,7 +4073,7 @@
       <c r="D44" s="1">
         <v>3</v>
       </c>
-      <c r="F44" s="12"/>
+      <c r="F44" s="11"/>
       <c r="K44" s="1" t="s">
         <v>190</v>
       </c>
@@ -4088,7 +4088,7 @@
       <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="F45" s="12"/>
+      <c r="F45" s="11"/>
       <c r="K45" s="1" t="s">
         <v>192</v>
       </c>
@@ -4103,7 +4103,7 @@
       <c r="D46" s="1">
         <v>1</v>
       </c>
-      <c r="F46" s="12"/>
+      <c r="F46" s="11"/>
       <c r="K46" s="1" t="s">
         <v>194</v>
       </c>
@@ -4118,7 +4118,7 @@
       <c r="D47" s="1">
         <v>4</v>
       </c>
-      <c r="F47" s="12"/>
+      <c r="F47" s="11"/>
       <c r="K47" s="1" t="s">
         <v>196</v>
       </c>
@@ -4133,7 +4133,7 @@
       <c r="D48" s="1">
         <v>1</v>
       </c>
-      <c r="F48" s="12"/>
+      <c r="F48" s="11"/>
       <c r="K48" s="1" t="s">
         <v>198</v>
       </c>
@@ -4148,7 +4148,7 @@
       <c r="D49" s="1">
         <v>1</v>
       </c>
-      <c r="F49" s="12"/>
+      <c r="F49" s="11"/>
       <c r="K49" s="1" t="s">
         <v>146</v>
       </c>
@@ -4163,7 +4163,7 @@
       <c r="D50" s="1">
         <v>1</v>
       </c>
-      <c r="F50" s="12"/>
+      <c r="F50" s="11"/>
       <c r="K50" s="1" t="s">
         <v>78</v>
       </c>
@@ -4178,16 +4178,16 @@
       <c r="D51" s="1">
         <v>1</v>
       </c>
-      <c r="F51" s="12"/>
+      <c r="F51" s="11"/>
       <c r="K51" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="L51" s="14" t="s">
+      <c r="L51" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="52" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F52" s="12"/>
+      <c r="F52" s="11"/>
       <c r="K52" s="1" t="s">
         <v>203</v>
       </c>
@@ -4196,7 +4196,7 @@
       </c>
     </row>
     <row r="53" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F53" s="12"/>
+      <c r="F53" s="11"/>
       <c r="K53" s="1" t="s">
         <v>204</v>
       </c>
@@ -4205,7 +4205,7 @@
       </c>
     </row>
     <row r="54" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F54" s="12"/>
+      <c r="F54" s="11"/>
       <c r="K54" s="1" t="s">
         <v>205</v>
       </c>
@@ -4214,7 +4214,7 @@
       </c>
     </row>
     <row r="55" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F55" s="12"/>
+      <c r="F55" s="11"/>
       <c r="K55" s="1" t="s">
         <v>206</v>
       </c>
@@ -4223,7 +4223,7 @@
       </c>
     </row>
     <row r="56" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F56" s="12"/>
+      <c r="F56" s="11"/>
       <c r="K56" s="1" t="s">
         <v>207</v>
       </c>
@@ -4232,7 +4232,7 @@
       </c>
     </row>
     <row r="57" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F57" s="12"/>
+      <c r="F57" s="11"/>
       <c r="K57" s="1" t="s">
         <v>208</v>
       </c>
@@ -4241,7 +4241,7 @@
       </c>
     </row>
     <row r="58" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F58" s="12"/>
+      <c r="F58" s="11"/>
       <c r="K58" s="1" t="s">
         <v>209</v>
       </c>
@@ -4250,7 +4250,7 @@
       </c>
     </row>
     <row r="59" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F59" s="12"/>
+      <c r="F59" s="11"/>
       <c r="K59" s="1" t="s">
         <v>210</v>
       </c>
@@ -4259,7 +4259,7 @@
       </c>
     </row>
     <row r="60" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F60" s="12"/>
+      <c r="F60" s="11"/>
       <c r="K60" s="1" t="s">
         <v>211</v>
       </c>
@@ -4268,7 +4268,7 @@
       </c>
     </row>
     <row r="61" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F61" s="12"/>
+      <c r="F61" s="11"/>
       <c r="K61" s="1" t="s">
         <v>212</v>
       </c>
@@ -4277,7 +4277,7 @@
       </c>
     </row>
     <row r="62" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F62" s="12"/>
+      <c r="F62" s="11"/>
       <c r="K62" s="1" t="s">
         <v>213</v>
       </c>
@@ -4286,7 +4286,7 @@
       </c>
     </row>
     <row r="63" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F63" s="12"/>
+      <c r="F63" s="11"/>
       <c r="K63" s="1" t="s">
         <v>214</v>
       </c>
@@ -4295,7 +4295,7 @@
       </c>
     </row>
     <row r="64" spans="3:12" ht="15.75" customHeight="1">
-      <c r="F64" s="12"/>
+      <c r="F64" s="11"/>
       <c r="K64" s="1" t="s">
         <v>215</v>
       </c>
@@ -4304,7 +4304,7 @@
       </c>
     </row>
     <row r="65" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F65" s="12"/>
+      <c r="F65" s="11"/>
       <c r="K65" s="1" t="s">
         <v>216</v>
       </c>
@@ -4313,7 +4313,7 @@
       </c>
     </row>
     <row r="66" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F66" s="12"/>
+      <c r="F66" s="11"/>
       <c r="K66" s="1" t="s">
         <v>217</v>
       </c>
@@ -4325,7 +4325,7 @@
       </c>
     </row>
     <row r="67" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F67" s="12"/>
+      <c r="F67" s="11"/>
       <c r="K67" s="1" t="s">
         <v>218</v>
       </c>
@@ -4334,7 +4334,7 @@
       </c>
     </row>
     <row r="68" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F68" s="12"/>
+      <c r="F68" s="11"/>
       <c r="K68" s="1" t="s">
         <v>219</v>
       </c>
@@ -4346,7 +4346,7 @@
       </c>
     </row>
     <row r="69" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F69" s="12"/>
+      <c r="F69" s="11"/>
       <c r="K69" s="1" t="s">
         <v>221</v>
       </c>
@@ -4355,7 +4355,7 @@
       </c>
     </row>
     <row r="70" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F70" s="12"/>
+      <c r="F70" s="11"/>
       <c r="K70" s="1" t="s">
         <v>222</v>
       </c>
@@ -4364,7 +4364,7 @@
       </c>
     </row>
     <row r="71" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F71" s="12"/>
+      <c r="F71" s="11"/>
       <c r="K71" s="1" t="s">
         <v>223</v>
       </c>
@@ -4373,7 +4373,7 @@
       </c>
     </row>
     <row r="72" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F72" s="12"/>
+      <c r="F72" s="11"/>
       <c r="K72" s="1" t="s">
         <v>224</v>
       </c>
@@ -4382,7 +4382,7 @@
       </c>
     </row>
     <row r="73" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F73" s="12"/>
+      <c r="F73" s="11"/>
       <c r="K73" s="1" t="s">
         <v>225</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
     </row>
     <row r="74" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F74" s="12"/>
+      <c r="F74" s="11"/>
       <c r="K74" s="1" t="s">
         <v>226</v>
       </c>
@@ -4400,7 +4400,7 @@
       </c>
     </row>
     <row r="75" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F75" s="12"/>
+      <c r="F75" s="11"/>
       <c r="K75" s="1" t="s">
         <v>227</v>
       </c>
@@ -4409,7 +4409,7 @@
       </c>
     </row>
     <row r="76" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F76" s="12"/>
+      <c r="F76" s="11"/>
       <c r="K76" s="1" t="s">
         <v>228</v>
       </c>
@@ -4418,7 +4418,7 @@
       </c>
     </row>
     <row r="77" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F77" s="12"/>
+      <c r="F77" s="11"/>
       <c r="K77" s="1" t="s">
         <v>229</v>
       </c>
@@ -4427,7 +4427,7 @@
       </c>
     </row>
     <row r="78" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F78" s="12"/>
+      <c r="F78" s="11"/>
       <c r="K78" s="1" t="s">
         <v>230</v>
       </c>
@@ -4436,7 +4436,7 @@
       </c>
     </row>
     <row r="79" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F79" s="12"/>
+      <c r="F79" s="11"/>
       <c r="K79" s="1" t="s">
         <v>231</v>
       </c>
@@ -4445,7 +4445,7 @@
       </c>
     </row>
     <row r="80" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F80" s="12"/>
+      <c r="F80" s="11"/>
       <c r="K80" s="1" t="s">
         <v>232</v>
       </c>
@@ -4457,7 +4457,7 @@
       </c>
     </row>
     <row r="81" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F81" s="12"/>
+      <c r="F81" s="11"/>
       <c r="K81" s="1" t="s">
         <v>233</v>
       </c>
@@ -4466,7 +4466,7 @@
       </c>
     </row>
     <row r="82" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F82" s="12"/>
+      <c r="F82" s="11"/>
       <c r="K82" s="1" t="s">
         <v>234</v>
       </c>
@@ -4475,7 +4475,7 @@
       </c>
     </row>
     <row r="83" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F83" s="12"/>
+      <c r="F83" s="11"/>
       <c r="K83" s="1" t="s">
         <v>235</v>
       </c>
@@ -4484,7 +4484,7 @@
       </c>
     </row>
     <row r="84" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F84" s="12"/>
+      <c r="F84" s="11"/>
       <c r="K84" s="1" t="s">
         <v>236</v>
       </c>
@@ -4493,7 +4493,7 @@
       </c>
     </row>
     <row r="85" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F85" s="12"/>
+      <c r="F85" s="11"/>
       <c r="K85" s="1" t="s">
         <v>237</v>
       </c>
@@ -4502,7 +4502,7 @@
       </c>
     </row>
     <row r="86" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F86" s="12"/>
+      <c r="F86" s="11"/>
       <c r="K86" s="1" t="s">
         <v>238</v>
       </c>
@@ -4511,7 +4511,7 @@
       </c>
     </row>
     <row r="87" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F87" s="12"/>
+      <c r="F87" s="11"/>
       <c r="K87" s="1" t="s">
         <v>239</v>
       </c>
@@ -4520,7 +4520,7 @@
       </c>
     </row>
     <row r="88" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F88" s="12"/>
+      <c r="F88" s="11"/>
       <c r="K88" s="1" t="s">
         <v>240</v>
       </c>
@@ -4529,7 +4529,7 @@
       </c>
     </row>
     <row r="89" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F89" s="12"/>
+      <c r="F89" s="11"/>
       <c r="K89" s="1" t="s">
         <v>241</v>
       </c>
@@ -4538,7 +4538,7 @@
       </c>
     </row>
     <row r="90" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F90" s="12"/>
+      <c r="F90" s="11"/>
       <c r="K90" s="1" t="s">
         <v>242</v>
       </c>
@@ -4547,7 +4547,7 @@
       </c>
     </row>
     <row r="91" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F91" s="12"/>
+      <c r="F91" s="11"/>
       <c r="K91" s="1" t="s">
         <v>243</v>
       </c>
@@ -4559,7 +4559,7 @@
       </c>
     </row>
     <row r="92" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F92" s="12"/>
+      <c r="F92" s="11"/>
       <c r="K92" s="1" t="s">
         <v>244</v>
       </c>
@@ -4568,7 +4568,7 @@
       </c>
     </row>
     <row r="93" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F93" s="12"/>
+      <c r="F93" s="11"/>
       <c r="K93" s="1" t="s">
         <v>245</v>
       </c>
@@ -4577,7 +4577,7 @@
       </c>
     </row>
     <row r="94" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F94" s="12"/>
+      <c r="F94" s="11"/>
       <c r="K94" s="1" t="s">
         <v>246</v>
       </c>
@@ -4586,7 +4586,7 @@
       </c>
     </row>
     <row r="95" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F95" s="12"/>
+      <c r="F95" s="11"/>
       <c r="K95" s="1" t="s">
         <v>247</v>
       </c>
@@ -4595,7 +4595,7 @@
       </c>
     </row>
     <row r="96" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F96" s="12"/>
+      <c r="F96" s="11"/>
       <c r="K96" s="1" t="s">
         <v>248</v>
       </c>
@@ -4604,7 +4604,7 @@
       </c>
     </row>
     <row r="97" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F97" s="12"/>
+      <c r="F97" s="11"/>
       <c r="K97" s="1" t="s">
         <v>249</v>
       </c>
@@ -4613,7 +4613,7 @@
       </c>
     </row>
     <row r="98" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F98" s="12"/>
+      <c r="F98" s="11"/>
       <c r="K98" s="1" t="s">
         <v>250</v>
       </c>
@@ -4622,7 +4622,7 @@
       </c>
     </row>
     <row r="99" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F99" s="12"/>
+      <c r="F99" s="11"/>
       <c r="K99" s="1" t="s">
         <v>251</v>
       </c>
@@ -4631,7 +4631,7 @@
       </c>
     </row>
     <row r="100" spans="6:13" ht="15.75" customHeight="1">
-      <c r="F100" s="12"/>
+      <c r="F100" s="11"/>
       <c r="K100" s="1" t="s">
         <v>252</v>
       </c>

</xml_diff>